<commit_message>
fix maker create excel
</commit_message>
<xml_diff>
--- a/base/Maker/repair_maker.xlsx
+++ b/base/Maker/repair_maker.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
@@ -442,7 +442,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.85546875" customWidth="1" min="1" max="1"/>
-    <col width="37.28515625" customWidth="1" min="2" max="2"/>
+    <col width="59.28515625" customWidth="1" min="2" max="2"/>
     <col width="21.85546875" customWidth="1" min="3" max="3"/>
     <col width="24.28515625" customWidth="1" min="4" max="4"/>
     <col width="28.140625" customWidth="1" min="5" max="5"/>
@@ -534,68 +534,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>проверка на "баги"  "ковычки"</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="n"/>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>Адлер</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t>ЭЛСИЭЛ</t>
-        </is>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>44606</v>
-      </c>
-      <c r="G3" s="4" t="n"/>
-      <c r="H3" s="4" t="n"/>
-      <c r="I3" s="4" t="inlineStr">
-        <is>
-          <t>ожидает</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>проверка на "баги"  "ковычки"</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Адлер</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>ЭЛСИЭЛ</t>
-        </is>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>44603</v>
-      </c>
-      <c r="G4" s="4" t="n"/>
-      <c r="H4" s="4" t="n"/>
-      <c r="I4" s="4" t="inlineStr">
-        <is>
-          <t>ожидает</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>